<commit_message>
RITM0167688 - RPA MIGRATION for Project Catalyst (all modifications for RPA in line to SAP Upgrade).
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a9005130_adm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEFC796-618D-464A-9E32-C8624CF1A07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -212,9 +213,6 @@
     <t>FilterName2</t>
   </si>
   <si>
-    <t>JE Created By</t>
-  </si>
-  <si>
     <t>InputFilterValue2</t>
   </si>
   <si>
@@ -374,14 +372,17 @@
     <t>SmallDelay</t>
   </si>
   <si>
-    <t>https://launchpad.orica.net/fiori#Shell-home</t>
+    <t>https://launchpad-dt.orica.net/fiori#Shell-home</t>
+  </si>
+  <si>
+    <t>Journal Entry Created By</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -404,6 +405,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9"/>
@@ -429,23 +436,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -757,11 +767,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -828,10 +838,10 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="C4" s="4"/>
     </row>
@@ -841,7 +851,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>22</v>
@@ -875,167 +885,167 @@
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>79</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
+        <v>78</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" t="s">
         <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" t="s">
         <v>71</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
         <v>73</v>
-      </c>
-      <c r="B19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>74</v>
+      </c>
+      <c r="B20" t="s">
         <v>75</v>
-      </c>
-      <c r="B20" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B21" t="s">
         <v>77</v>
-      </c>
-      <c r="B21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" t="s">
         <v>111</v>
-      </c>
-      <c r="B23" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
+        <v>108</v>
+      </c>
+      <c r="B24" t="s">
         <v>109</v>
-      </c>
-      <c r="B24" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" t="s">
         <v>107</v>
-      </c>
-      <c r="B25" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C28" s="3"/>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
         <v>86</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B34" t="s">
         <v>99</v>
       </c>
-      <c r="B34" t="s">
-        <v>100</v>
-      </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B35" s="6"/>
+      <c r="B35" s="7"/>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2009,17 +2019,23 @@
     <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1" location="Shell-home" xr:uid="{1BD81B70-B676-4913-9681-47932565C4C4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z992"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2077,13 +2093,13 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="45">
@@ -2216,10 +2232,10 @@
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
         <v>96</v>
-      </c>
-      <c r="B20" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2267,10 +2283,10 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
         <v>69</v>
-      </c>
-      <c r="B29" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
@@ -2295,15 +2311,15 @@
         <v>61</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="14.25" customHeight="1">
       <c r="A34" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" t="s">
         <v>63</v>
-      </c>
-      <c r="B34" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3267,11 +3283,14 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3324,57 +3343,57 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
@@ -4375,5 +4394,8 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RITM0167688 - Update code in line to SAP Upgrade
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessica.lara\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEFC796-618D-464A-9E32-C8624CF1A07B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A97DA3-DADE-4BAD-81E9-A2CCC85081BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
     <t>SmallDelay</t>
   </si>
   <si>
-    <t>https://launchpad-dt.orica.net/fiori#Shell-home</t>
+    <t>https://launchpad.orica.net/fiori#Shell-home</t>
   </si>
   <si>
     <t>Journal Entry Created By</t>
@@ -382,7 +382,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -405,12 +405,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="9"/>
@@ -436,26 +430,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="7">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,8 +761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -887,7 +878,7 @@
       <c r="A12" t="s">
         <v>78</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1045,7 +1036,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B35" s="7"/>
+      <c r="B35" s="6"/>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2019,14 +2010,8 @@
     <row r="1005" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
-  <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1" location="Shell-home" xr:uid="{1BD81B70-B676-4913-9681-47932565C4C4}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2035,7 +2020,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3283,9 +3268,6 @@
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
 
@@ -4394,8 +4376,5 @@
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Arial"&amp;10&amp;K000000 General</oddFooter>
-  </headerFooter>
 </worksheet>
 </file>
</xml_diff>